<commit_message>
Updated 7 week plan
7 week plan updated, moved vehicle map to top of S items and updated item descriptions.
</commit_message>
<xml_diff>
--- a/7 Week Plan.xlsx
+++ b/7 Week Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\OneDrive\Documents\Uni\Year 3\Group Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{268891BB-4967-4F1B-B592-98A6798DCFA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF37531F-4315-4E42-A73E-2605616A1766}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{268891BB-4967-4F1B-B592-98A6798DCFA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{14D9C62A-80FA-49E0-963A-D6D7C3CC9346}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3D1D16ED-B982-4B46-911F-05DE94ADF26F}"/>
   </bookViews>
@@ -120,15 +120,6 @@
     <t>Allows users to check vehicle out from work place. Select car to be delivered.</t>
   </si>
   <si>
-    <t>Allow users to check and take evidence of the current condition of the vehicle.</t>
-  </si>
-  <si>
-    <t>Allow users to check and take evidence of the current condition of the vehicle at delivery.</t>
-  </si>
-  <si>
-    <t>Allow users to check and take evidence of the current condition of the vehicle at collection.</t>
-  </si>
-  <si>
     <t>MoSCoW:</t>
   </si>
   <si>
@@ -211,6 +202,15 @@
   </si>
   <si>
     <t>Allow user to register damages viewed through photo comparison.</t>
+  </si>
+  <si>
+    <t>Allow users to mark a vehicle as delivered.</t>
+  </si>
+  <si>
+    <t>Allow users to mark a vehicle as collected.</t>
+  </si>
+  <si>
+    <t>Allow users to update stored customer information.</t>
   </si>
 </sst>
 </file>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F925CB74-4A21-49DD-9959-D892FD87F18E}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -608,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -627,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
@@ -649,7 +649,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>28</v>
@@ -663,7 +663,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -677,10 +677,10 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -691,10 +691,10 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,10 +705,10 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>
@@ -733,7 +733,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -747,15 +747,15 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,13 +766,13 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -780,7 +780,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E21" t="s">
         <v>26</v>
@@ -788,92 +788,92 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C22">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C25">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C26">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -881,27 +881,27 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" t="s">
         <v>41</v>
-      </c>
-      <c r="C34" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" t="s">
-        <v>45</v>
-      </c>
-      <c r="G34" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -929,7 +929,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -949,7 +949,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D37">
         <v>5</v>
@@ -969,7 +969,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D38">
         <v>6</v>
@@ -989,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D39">
         <v>9</v>
@@ -1009,7 +1009,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D40">
         <v>10</v>
@@ -1029,13 +1029,13 @@
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D41">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E41">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F41">
         <v>12</v>
@@ -1046,5 +1046,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>